<commit_message>
Added Keyvault mertic table
</commit_message>
<xml_diff>
--- a/CRM Solution Manager/Release/KeyVault/AzureKeyVaultNames.xlsx
+++ b/CRM Solution Manager/Release/KeyVault/AzureKeyVaultNames.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-ynaresh\source\repos\DynamicsPOC5\CRM Solution Manager\Release\KeyVault\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-ynaresh\source\repos\DynamicsPOC\CRM Solution Manager\Release\KeyVault\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2169A583-0EAC-42F0-BF5A-D109AD0B6A3C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5806B6E-51B4-4013-80F4-2644A605167C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{954886C5-4D1A-4ACB-BA8C-D15138D5C5AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{954886C5-4D1A-4ACB-BA8C-D15138D5C5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Key-Vault secrets" sheetId="2" r:id="rId2"/>
-    <sheet name="Configuration settings" sheetId="3" r:id="rId3"/>
+    <sheet name="KeyVaults Usage" sheetId="4" r:id="rId3"/>
+    <sheet name="Configuration settings" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="98">
   <si>
     <t>ClientApplicationSecret</t>
   </si>
@@ -384,12 +385,42 @@
   <si>
     <t>in Pipilines we are using the these color secrets</t>
   </si>
+  <si>
+    <t>KeyVault Secret</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Azure Function App settings</t>
+  </si>
+  <si>
+    <t>Azure Function Code</t>
+  </si>
+  <si>
+    <t>Devops Build pipeline</t>
+  </si>
+  <si>
+    <t>Devops Release Pipeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> û</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>û</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ü</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,8 +461,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,6 +496,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -570,6 +619,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1108,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25B193B-9A8B-49E8-9D23-A31F8139F4B4}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1349,6 +1410,309 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB24A900-5F8F-4C6A-AC20-2090EE646726}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA44A09-FB88-462E-A9D9-8257E778990C}">
   <dimension ref="A1:B19"/>
   <sheetViews>

</xml_diff>